<commit_message>
Change to others mistakes
</commit_message>
<xml_diff>
--- a/data/misused_bar_graph_figures/nat_biotechnol/log/annotation.xlsx
+++ b/data/misused_bar_graph_figures/nat_biotechnol/log/annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Files/2023-2028-UC_Berkeley/_landry-lab/research-project/local/misused-bar-graphs/data/misused_bar_graph_figures/nat_biotechnol/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EAF7E7-E48F-914D-8845-1212E113C06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DAFB53-F526-6049-A8F8-402823D6128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="18800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="500" windowWidth="18800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="237">
   <si>
     <t>DOI</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Human CD45+ cells per gram</t>
   </si>
   <si>
-    <t>Fold change</t>
-  </si>
-  <si>
     <t>Number of spectra factors</t>
   </si>
   <si>
@@ -728,9 +725,6 @@
   </si>
   <si>
     <t>10.1038:s41587-023-01931-4_log_fig4</t>
-  </si>
-  <si>
-    <t>10.1038:s41587-023-01931-4_log_fig5</t>
   </si>
   <si>
     <t>Others</t>
@@ -1137,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H62" zoomScale="200" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,7 +1146,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1170,24 +1164,24 @@
         <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1205,24 +1199,24 @@
         <v>54</v>
       </c>
       <c r="G2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" t="s">
         <v>122</v>
       </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
       <c r="I2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1240,24 +1234,24 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
         <v>122</v>
       </c>
-      <c r="H3" t="s">
-        <v>123</v>
-      </c>
       <c r="I3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1275,24 +1269,24 @@
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1310,24 +1304,24 @@
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1345,24 +1339,24 @@
         <v>57</v>
       </c>
       <c r="G6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" t="s">
         <v>122</v>
       </c>
-      <c r="H6" t="s">
-        <v>123</v>
-      </c>
       <c r="I6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1380,24 +1374,24 @@
         <v>58</v>
       </c>
       <c r="G7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" t="s">
         <v>122</v>
       </c>
-      <c r="H7" t="s">
-        <v>123</v>
-      </c>
       <c r="I7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1415,24 +1409,24 @@
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1450,24 +1444,24 @@
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" t="s">
         <v>130</v>
       </c>
-      <c r="I9" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" t="s">
-        <v>131</v>
-      </c>
       <c r="K9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1485,24 +1479,24 @@
         <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" t="s">
         <v>130</v>
       </c>
-      <c r="I10" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" t="s">
-        <v>131</v>
-      </c>
       <c r="K10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1520,24 +1514,24 @@
         <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1555,24 +1549,24 @@
         <v>62</v>
       </c>
       <c r="G12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" t="s">
         <v>122</v>
       </c>
-      <c r="H12" t="s">
-        <v>123</v>
-      </c>
       <c r="I12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1590,24 +1584,24 @@
         <v>62</v>
       </c>
       <c r="G13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" t="s">
         <v>122</v>
       </c>
-      <c r="H13" t="s">
-        <v>123</v>
-      </c>
       <c r="I13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1625,24 +1619,24 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1660,24 +1654,24 @@
         <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1695,24 +1689,24 @@
         <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -1730,24 +1724,24 @@
         <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -1765,24 +1759,24 @@
         <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1800,24 +1794,24 @@
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1835,24 +1829,24 @@
         <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1870,24 +1864,24 @@
         <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -1905,24 +1899,24 @@
         <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -1940,24 +1934,24 @@
         <v>72</v>
       </c>
       <c r="G23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -1975,10 +1969,10 @@
         <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I24" t="s">
         <v>67</v>
@@ -1987,12 +1981,12 @@
         <v>67</v>
       </c>
       <c r="K24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -2010,10 +2004,10 @@
         <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I25" t="s">
         <v>67</v>
@@ -2022,12 +2016,12 @@
         <v>67</v>
       </c>
       <c r="K25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -2045,10 +2039,10 @@
         <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" t="s">
         <v>67</v>
@@ -2057,12 +2051,12 @@
         <v>67</v>
       </c>
       <c r="K26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
@@ -2080,10 +2074,10 @@
         <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I27" t="s">
         <v>67</v>
@@ -2092,12 +2086,12 @@
         <v>67</v>
       </c>
       <c r="K27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -2115,10 +2109,10 @@
         <v>67</v>
       </c>
       <c r="G28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" t="s">
         <v>67</v>
@@ -2127,12 +2121,12 @@
         <v>67</v>
       </c>
       <c r="K28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -2150,10 +2144,10 @@
         <v>67</v>
       </c>
       <c r="G29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I29" t="s">
         <v>67</v>
@@ -2162,12 +2156,12 @@
         <v>67</v>
       </c>
       <c r="K29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -2185,10 +2179,10 @@
         <v>67</v>
       </c>
       <c r="G30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I30" t="s">
         <v>67</v>
@@ -2197,12 +2191,12 @@
         <v>67</v>
       </c>
       <c r="K30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -2220,10 +2214,10 @@
         <v>67</v>
       </c>
       <c r="G31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I31" t="s">
         <v>67</v>
@@ -2232,12 +2226,12 @@
         <v>67</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -2255,24 +2249,24 @@
         <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -2290,24 +2284,24 @@
         <v>74</v>
       </c>
       <c r="G33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -2325,24 +2319,24 @@
         <v>74</v>
       </c>
       <c r="G34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
@@ -2360,24 +2354,24 @@
         <v>74</v>
       </c>
       <c r="G35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
@@ -2395,24 +2389,24 @@
         <v>74</v>
       </c>
       <c r="G36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
@@ -2430,24 +2424,24 @@
         <v>74</v>
       </c>
       <c r="G37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
@@ -2465,24 +2459,24 @@
         <v>75</v>
       </c>
       <c r="G38" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" t="s">
         <v>122</v>
       </c>
-      <c r="H38" t="s">
-        <v>123</v>
-      </c>
       <c r="I38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
@@ -2500,24 +2494,24 @@
         <v>75</v>
       </c>
       <c r="G39" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39" t="s">
         <v>122</v>
       </c>
-      <c r="H39" t="s">
-        <v>123</v>
-      </c>
       <c r="I39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
@@ -2535,24 +2529,24 @@
         <v>75</v>
       </c>
       <c r="G40" t="s">
+        <v>121</v>
+      </c>
+      <c r="H40" t="s">
         <v>122</v>
       </c>
-      <c r="H40" t="s">
-        <v>123</v>
-      </c>
       <c r="I40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -2570,24 +2564,24 @@
         <v>75</v>
       </c>
       <c r="G41" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" t="s">
         <v>122</v>
       </c>
-      <c r="H41" t="s">
-        <v>123</v>
-      </c>
       <c r="I41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
@@ -2605,24 +2599,24 @@
         <v>76</v>
       </c>
       <c r="G42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
@@ -2640,24 +2634,24 @@
         <v>77</v>
       </c>
       <c r="G43" t="s">
+        <v>121</v>
+      </c>
+      <c r="H43" t="s">
         <v>122</v>
       </c>
-      <c r="H43" t="s">
-        <v>123</v>
-      </c>
       <c r="I43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
@@ -2675,24 +2669,24 @@
         <v>78</v>
       </c>
       <c r="G44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B45" t="s">
         <v>34</v>
@@ -2710,10 +2704,10 @@
         <v>79</v>
       </c>
       <c r="G45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I45" t="s">
         <v>67</v>
@@ -2722,12 +2716,12 @@
         <v>67</v>
       </c>
       <c r="K45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B46" t="s">
         <v>34</v>
@@ -2742,13 +2736,13 @@
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I46" t="s">
         <v>67</v>
@@ -2757,12 +2751,12 @@
         <v>67</v>
       </c>
       <c r="K46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B47" t="s">
         <v>34</v>
@@ -2777,13 +2771,13 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I47" t="s">
         <v>67</v>
@@ -2792,12 +2786,12 @@
         <v>67</v>
       </c>
       <c r="K47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" t="s">
         <v>35</v>
@@ -2815,24 +2809,24 @@
         <v>80</v>
       </c>
       <c r="G48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H48" t="s">
+        <v>129</v>
+      </c>
+      <c r="I48" t="s">
+        <v>131</v>
+      </c>
+      <c r="J48" t="s">
         <v>130</v>
       </c>
-      <c r="I48" t="s">
-        <v>132</v>
-      </c>
-      <c r="J48" t="s">
-        <v>131</v>
-      </c>
       <c r="K48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -2850,24 +2844,24 @@
         <v>81</v>
       </c>
       <c r="G49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J49" t="s">
         <v>67</v>
       </c>
       <c r="K49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B50" t="s">
         <v>36</v>
@@ -2885,24 +2879,24 @@
         <v>82</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J50" t="s">
         <v>67</v>
       </c>
       <c r="K50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
         <v>37</v>
@@ -2920,24 +2914,24 @@
         <v>83</v>
       </c>
       <c r="G51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I51" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J51" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B52" t="s">
         <v>37</v>
@@ -2955,24 +2949,24 @@
         <v>83</v>
       </c>
       <c r="G52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B53" t="s">
         <v>37</v>
@@ -2990,24 +2984,24 @@
         <v>84</v>
       </c>
       <c r="G53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
         <v>38</v>
@@ -3025,10 +3019,10 @@
         <v>85</v>
       </c>
       <c r="G54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I54" t="s">
         <v>67</v>
@@ -3037,12 +3031,12 @@
         <v>67</v>
       </c>
       <c r="K54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B55" t="s">
         <v>38</v>
@@ -3060,10 +3054,10 @@
         <v>87</v>
       </c>
       <c r="G55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I55" t="s">
         <v>67</v>
@@ -3072,12 +3066,12 @@
         <v>67</v>
       </c>
       <c r="K55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
         <v>39</v>
@@ -3095,24 +3089,24 @@
         <v>86</v>
       </c>
       <c r="G56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
         <v>39</v>
@@ -3130,24 +3124,24 @@
         <v>86</v>
       </c>
       <c r="G57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B58" t="s">
         <v>39</v>
@@ -3165,24 +3159,24 @@
         <v>86</v>
       </c>
       <c r="G58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B59" t="s">
         <v>39</v>
@@ -3200,24 +3194,24 @@
         <v>86</v>
       </c>
       <c r="G59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B60" t="s">
         <v>39</v>
@@ -3235,24 +3229,24 @@
         <v>86</v>
       </c>
       <c r="G60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B61" t="s">
         <v>39</v>
@@ -3270,24 +3264,24 @@
         <v>86</v>
       </c>
       <c r="G61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B62" t="s">
         <v>39</v>
@@ -3305,24 +3299,24 @@
         <v>86</v>
       </c>
       <c r="G62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B63" t="s">
         <v>39</v>
@@ -3340,24 +3334,24 @@
         <v>86</v>
       </c>
       <c r="G63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
@@ -3375,24 +3369,24 @@
         <v>86</v>
       </c>
       <c r="G64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B65" t="s">
         <v>40</v>
@@ -3410,24 +3404,24 @@
         <v>88</v>
       </c>
       <c r="G65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I65" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B66" t="s">
         <v>40</v>
@@ -3445,24 +3439,24 @@
         <v>89</v>
       </c>
       <c r="G66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I66" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B67" t="s">
         <v>40</v>
@@ -3480,24 +3474,24 @@
         <v>89</v>
       </c>
       <c r="G67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I67" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
         <v>40</v>
@@ -3515,24 +3509,24 @@
         <v>89</v>
       </c>
       <c r="G68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I68" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B69" t="s">
         <v>41</v>
@@ -3550,24 +3544,24 @@
         <v>90</v>
       </c>
       <c r="G69" t="s">
+        <v>121</v>
+      </c>
+      <c r="H69" t="s">
         <v>122</v>
       </c>
-      <c r="H69" t="s">
-        <v>123</v>
-      </c>
       <c r="I69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
@@ -3585,24 +3579,24 @@
         <v>91</v>
       </c>
       <c r="G70" t="s">
+        <v>121</v>
+      </c>
+      <c r="H70" t="s">
         <v>122</v>
       </c>
-      <c r="H70" t="s">
-        <v>123</v>
-      </c>
       <c r="I70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B71" t="s">
         <v>41</v>
@@ -3620,24 +3614,24 @@
         <v>91</v>
       </c>
       <c r="G71" t="s">
+        <v>121</v>
+      </c>
+      <c r="H71" t="s">
         <v>122</v>
       </c>
-      <c r="H71" t="s">
-        <v>123</v>
-      </c>
       <c r="I71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B72" t="s">
         <v>42</v>
@@ -3655,24 +3649,24 @@
         <v>92</v>
       </c>
       <c r="G72" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J72" t="s">
         <v>67</v>
       </c>
       <c r="K72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B73" t="s">
         <v>42</v>
@@ -3690,24 +3684,24 @@
         <v>101</v>
       </c>
       <c r="G73" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J73" t="s">
         <v>67</v>
       </c>
       <c r="K73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
         <v>42</v>
@@ -3725,24 +3719,24 @@
         <v>102</v>
       </c>
       <c r="G74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J74" t="s">
         <v>67</v>
       </c>
       <c r="K74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B75" t="s">
         <v>42</v>
@@ -3760,24 +3754,24 @@
         <v>103</v>
       </c>
       <c r="G75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J75" t="s">
         <v>67</v>
       </c>
       <c r="K75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
         <v>42</v>
@@ -3795,24 +3789,24 @@
         <v>104</v>
       </c>
       <c r="G76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J76" t="s">
         <v>67</v>
       </c>
       <c r="K76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
@@ -3830,24 +3824,24 @@
         <v>105</v>
       </c>
       <c r="G77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J77" t="s">
         <v>67</v>
       </c>
       <c r="K77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B78" t="s">
         <v>42</v>
@@ -3865,24 +3859,24 @@
         <v>106</v>
       </c>
       <c r="G78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J78" t="s">
         <v>67</v>
       </c>
       <c r="K78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B79" t="s">
         <v>42</v>
@@ -3900,10 +3894,10 @@
         <v>107</v>
       </c>
       <c r="G79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I79" t="s">
         <v>67</v>
@@ -3912,12 +3906,12 @@
         <v>67</v>
       </c>
       <c r="K79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B80" t="s">
         <v>42</v>
@@ -3935,24 +3929,24 @@
         <v>108</v>
       </c>
       <c r="G80" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J80" t="s">
         <v>67</v>
       </c>
       <c r="K80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B81" t="s">
         <v>42</v>
@@ -3970,24 +3964,24 @@
         <v>109</v>
       </c>
       <c r="G81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J81" t="s">
         <v>67</v>
       </c>
       <c r="K81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
         <v>42</v>
@@ -4005,24 +3999,24 @@
         <v>110</v>
       </c>
       <c r="G82" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J82" t="s">
         <v>67</v>
       </c>
       <c r="K82" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B83" t="s">
         <v>42</v>
@@ -4040,24 +4034,24 @@
         <v>95</v>
       </c>
       <c r="G83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I83" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J83" t="s">
         <v>67</v>
       </c>
       <c r="K83" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B84" t="s">
         <v>42</v>
@@ -4075,24 +4069,24 @@
         <v>111</v>
       </c>
       <c r="G84" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I84" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J84" t="s">
         <v>67</v>
       </c>
       <c r="K84" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B85" t="s">
         <v>42</v>
@@ -4110,24 +4104,24 @@
         <v>112</v>
       </c>
       <c r="G85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H85" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J85" t="s">
         <v>67</v>
       </c>
       <c r="K85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B86" t="s">
         <v>42</v>
@@ -4145,10 +4139,10 @@
         <v>107</v>
       </c>
       <c r="G86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I86" t="s">
         <v>67</v>
@@ -4157,12 +4151,12 @@
         <v>67</v>
       </c>
       <c r="K86" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B87" t="s">
         <v>42</v>
@@ -4180,10 +4174,10 @@
         <v>107</v>
       </c>
       <c r="G87" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H87" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I87" t="s">
         <v>67</v>
@@ -4192,12 +4186,12 @@
         <v>67</v>
       </c>
       <c r="K87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B88" t="s">
         <v>42</v>
@@ -4215,24 +4209,24 @@
         <v>93</v>
       </c>
       <c r="G88" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H88" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J88" t="s">
         <v>67</v>
       </c>
       <c r="K88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B89" t="s">
         <v>42</v>
@@ -4250,24 +4244,24 @@
         <v>94</v>
       </c>
       <c r="G89" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H89" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I89" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J89" t="s">
         <v>67</v>
       </c>
       <c r="K89" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B90" t="s">
         <v>42</v>
@@ -4285,24 +4279,24 @@
         <v>96</v>
       </c>
       <c r="G90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H90" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I90" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J90" t="s">
         <v>67</v>
       </c>
       <c r="K90" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B91" t="s">
         <v>42</v>
@@ -4320,24 +4314,24 @@
         <v>97</v>
       </c>
       <c r="G91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I91" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J91" t="s">
         <v>67</v>
       </c>
       <c r="K91" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B92" t="s">
         <v>42</v>
@@ -4355,24 +4349,24 @@
         <v>98</v>
       </c>
       <c r="G92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I92" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J92" t="s">
         <v>67</v>
       </c>
       <c r="K92" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B93" t="s">
         <v>42</v>
@@ -4390,24 +4384,24 @@
         <v>99</v>
       </c>
       <c r="G93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H93" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J93" t="s">
         <v>67</v>
       </c>
       <c r="K93" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B94" t="s">
         <v>42</v>
@@ -4425,24 +4419,24 @@
         <v>100</v>
       </c>
       <c r="G94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I94" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J94" t="s">
         <v>67</v>
       </c>
       <c r="K94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
@@ -4457,13 +4451,13 @@
         <v>7</v>
       </c>
       <c r="F95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G95" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I95" t="s">
         <v>67</v>
@@ -4472,12 +4466,12 @@
         <v>67</v>
       </c>
       <c r="K95" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
@@ -4492,13 +4486,13 @@
         <v>7</v>
       </c>
       <c r="F96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G96" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I96" t="s">
         <v>67</v>
@@ -4507,12 +4501,12 @@
         <v>67</v>
       </c>
       <c r="K96" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
@@ -4527,13 +4521,13 @@
         <v>7</v>
       </c>
       <c r="F97" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I97" t="s">
         <v>67</v>
@@ -4542,12 +4536,12 @@
         <v>67</v>
       </c>
       <c r="K97" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
@@ -4562,13 +4556,13 @@
         <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H98" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I98" t="s">
         <v>67</v>
@@ -4577,42 +4571,7 @@
         <v>67</v>
       </c>
       <c r="K98" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B99" t="s">
-        <v>52</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E99" t="s">
-        <v>7</v>
-      </c>
-      <c r="F99" t="s">
-        <v>113</v>
-      </c>
-      <c r="G99" t="s">
-        <v>122</v>
-      </c>
-      <c r="H99" t="s">
-        <v>123</v>
-      </c>
-      <c r="I99" t="s">
-        <v>123</v>
-      </c>
-      <c r="J99" t="s">
-        <v>123</v>
-      </c>
-      <c r="K99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>